<commit_message>
Cleaned up Fish XLS file and metadata
</commit_message>
<xml_diff>
--- a/Data/Fish Indicator Species for EEP.xlsx
+++ b/Data/Fish Indicator Species for EEP.xlsx
@@ -5,24 +5,23 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Workspace\EEP\Docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Workspace\NC_DMS\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25065" windowHeight="9840" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25065" windowHeight="9840"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Piedmont" sheetId="3" r:id="rId3"/>
-    <sheet name="MACP" sheetId="4" r:id="rId4"/>
+    <sheet name="Master" sheetId="1" r:id="rId1"/>
+    <sheet name="Piedmont" sheetId="3" r:id="rId2"/>
+    <sheet name="MACP" sheetId="4" r:id="rId3"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="101">
   <si>
     <t>Level III Ecoregion</t>
   </si>
@@ -244,9 +243,6 @@
   </si>
   <si>
     <t>Cover</t>
-  </si>
-  <si>
-    <t>Common</t>
   </si>
   <si>
     <t>Scientific</t>
@@ -720,7 +716,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E47"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
@@ -1274,126 +1270,9 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:C13"/>
+  <dimension ref="A1:C13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7:XFD7"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="2" max="2" width="55.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="31.7109375" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B1" t="s">
-        <v>74</v>
-      </c>
-      <c r="C1" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="2" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B2" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="C2" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="3" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B3" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="C3" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="4" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B4" s="10" t="s">
-        <v>26</v>
-      </c>
-      <c r="C4" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="5" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B5" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="C5" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="6" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B6" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="C6" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="7" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B7" s="10" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="8" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B8" s="10" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="9" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B9" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="C9" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="10" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B10" s="10" t="s">
-        <v>18</v>
-      </c>
-      <c r="C10" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="11" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B11" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="C11" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="12" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B12" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="C12" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="13" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B13" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="C13" t="s">
-        <v>85</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C13"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
@@ -1406,13 +1285,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="12" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B1" s="12" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -1420,7 +1299,7 @@
         <v>13</v>
       </c>
       <c r="B2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -1428,7 +1307,7 @@
         <v>19</v>
       </c>
       <c r="B3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -1436,7 +1315,7 @@
         <v>26</v>
       </c>
       <c r="B4" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -1444,7 +1323,7 @@
         <v>17</v>
       </c>
       <c r="B5" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -1452,7 +1331,7 @@
         <v>16</v>
       </c>
       <c r="B6" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -1460,10 +1339,10 @@
         <v>14</v>
       </c>
       <c r="B7" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C7" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -1471,10 +1350,10 @@
         <v>57</v>
       </c>
       <c r="B8" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C8" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
@@ -1482,7 +1361,7 @@
         <v>21</v>
       </c>
       <c r="B9" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
@@ -1490,7 +1369,7 @@
         <v>18</v>
       </c>
       <c r="B10" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
@@ -1498,7 +1377,7 @@
         <v>15</v>
       </c>
       <c r="B11" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
@@ -1506,7 +1385,7 @@
         <v>12</v>
       </c>
       <c r="B12" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
@@ -1514,10 +1393,10 @@
         <v>20</v>
       </c>
       <c r="B13" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C13" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
   </sheetData>
@@ -1526,7 +1405,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B11"/>
   <sheetViews>
@@ -1542,10 +1421,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="12" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B1" s="12" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -1553,7 +1432,7 @@
         <v>22</v>
       </c>
       <c r="B2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -1561,7 +1440,7 @@
         <v>23</v>
       </c>
       <c r="B3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -1569,7 +1448,7 @@
         <v>72</v>
       </c>
       <c r="B4" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -1577,7 +1456,7 @@
         <v>24</v>
       </c>
       <c r="B5" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -1585,7 +1464,7 @@
         <v>71</v>
       </c>
       <c r="B6" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -1593,7 +1472,7 @@
         <v>25</v>
       </c>
       <c r="B7" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
@@ -1601,7 +1480,7 @@
         <v>26</v>
       </c>
       <c r="B8" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
@@ -1609,7 +1488,7 @@
         <v>27</v>
       </c>
       <c r="B9" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
@@ -1617,7 +1496,7 @@
         <v>28</v>
       </c>
       <c r="B10" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
@@ -1625,7 +1504,7 @@
         <v>29</v>
       </c>
       <c r="B11" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixed species names in MACP
</commit_message>
<xml_diff>
--- a/Data/Fish Indicator Species for EEP.xlsx
+++ b/Data/Fish Indicator Species for EEP.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25065" windowHeight="9840"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25065" windowHeight="9840" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Master" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="102">
   <si>
     <t>Level III Ecoregion</t>
   </si>
@@ -281,33 +281,6 @@
     <t>CommonName</t>
   </si>
   <si>
-    <t>Anguilla rostrata</t>
-  </si>
-  <si>
-    <t>Umbra pygmaea</t>
-  </si>
-  <si>
-    <t>Esox americanus</t>
-  </si>
-  <si>
-    <t>Notropis cummingsae;Notropis procne;Notropis chalybaeus;Notropis altipinnis</t>
-  </si>
-  <si>
-    <t>Erimyzon oblongus;Minytrema melanops</t>
-  </si>
-  <si>
-    <t>Noturus gyrinus</t>
-  </si>
-  <si>
-    <t>Acantharchus pomotis</t>
-  </si>
-  <si>
-    <t>Enneacanthus gloriosus</t>
-  </si>
-  <si>
-    <t>Etheostoma olmstedi</t>
-  </si>
-  <si>
     <t>Notropis_chlorocephalus</t>
   </si>
   <si>
@@ -324,6 +297,36 @@
   </si>
   <si>
     <t>AdditionalSpp</t>
+  </si>
+  <si>
+    <t>Anguilla_rostrata</t>
+  </si>
+  <si>
+    <t>Umbra_pygmaea</t>
+  </si>
+  <si>
+    <t>Notropis_cummingsae</t>
+  </si>
+  <si>
+    <t>Esox_americanus</t>
+  </si>
+  <si>
+    <t>Erimyzon_oblongus</t>
+  </si>
+  <si>
+    <t>Noturus_gyrinus</t>
+  </si>
+  <si>
+    <t>Acantharchus_pomotis</t>
+  </si>
+  <si>
+    <t>Enneacanthus_gloriosus</t>
+  </si>
+  <si>
+    <t>Notropis_procne;Notropis_chalybaeus;Notropis_altipinnis</t>
+  </si>
+  <si>
+    <t>Minytrema_melanops</t>
   </si>
 </sst>
 </file>
@@ -716,7 +719,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E47"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
@@ -1291,7 +1294,7 @@
         <v>74</v>
       </c>
       <c r="C1" t="s">
-        <v>100</v>
+        <v>91</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -1339,10 +1342,10 @@
         <v>14</v>
       </c>
       <c r="B7" t="s">
-        <v>97</v>
+        <v>88</v>
       </c>
       <c r="C7" t="s">
-        <v>95</v>
+        <v>86</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -1350,10 +1353,10 @@
         <v>57</v>
       </c>
       <c r="B8" t="s">
-        <v>98</v>
+        <v>89</v>
       </c>
       <c r="C8" t="s">
-        <v>96</v>
+        <v>87</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
@@ -1396,7 +1399,7 @@
         <v>84</v>
       </c>
       <c r="C13" t="s">
-        <v>99</v>
+        <v>90</v>
       </c>
     </row>
   </sheetData>
@@ -1407,75 +1410,85 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B11"/>
+  <dimension ref="A1:C11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="54.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="72.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="52.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="12" t="s">
         <v>85</v>
       </c>
       <c r="B1" s="12" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C1" s="12" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="10" t="s">
         <v>22</v>
       </c>
       <c r="B2" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="10" t="s">
         <v>23</v>
       </c>
       <c r="B3" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="10" t="s">
         <v>72</v>
       </c>
       <c r="B4" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+        <v>94</v>
+      </c>
+      <c r="C4" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="10" t="s">
         <v>24</v>
       </c>
       <c r="B5" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="10" t="s">
         <v>71</v>
       </c>
       <c r="B6" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+        <v>96</v>
+      </c>
+      <c r="C6" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="10" t="s">
         <v>25</v>
       </c>
       <c r="B7" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="10" t="s">
         <v>26</v>
       </c>
@@ -1483,31 +1496,32 @@
         <v>77</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="10" t="s">
         <v>27</v>
       </c>
       <c r="B9" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="10" t="s">
         <v>28</v>
       </c>
       <c r="B10" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="10" t="s">
         <v>29</v>
       </c>
       <c r="B11" t="s">
-        <v>94</v>
+        <v>84</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>